<commit_message>
Updated mapping excel for source field names
</commit_message>
<xml_diff>
--- a/solution/pybe/mappings/mappings.xlsx
+++ b/solution/pybe/mappings/mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Documents\DevStuff\RodoChallenge\solution\pybe\mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEAA2C9B-E78B-4029-8D82-91A840271889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F3F745-8F7C-48F3-B494-369CD754755C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CD695783-2CB4-46E3-A5D2-2BBECD8B6EC7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="81">
   <si>
     <t>dealership_id</t>
   </si>
@@ -273,6 +273,12 @@
   </si>
   <si>
     <t>|</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -288,12 +294,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -308,8 +320,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -785,7 +798,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,8 +850,8 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
+      <c r="B5" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -848,8 +861,8 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
+      <c r="B6" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1060,7 +1073,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Basic working solution * updated gitignore for excel locks * added fields to models * added table for validation errors * added db clear route to api
</commit_message>
<xml_diff>
--- a/solution/pybe/mappings/mappings.xlsx
+++ b/solution/pybe/mappings/mappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Documents\DevStuff\RodoChallenge\solution\pybe\mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F3F745-8F7C-48F3-B494-369CD754755C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2950835-84A5-4F6E-A075-FACE82C5EA48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CD695783-2CB4-46E3-A5D2-2BBECD8B6EC7}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{CD695783-2CB4-46E3-A5D2-2BBECD8B6EC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="83">
   <si>
     <t>dealership_id</t>
   </si>
@@ -279,6 +279,12 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>dealer_list_price</t>
+  </si>
+  <si>
+    <t>List Price</t>
   </si>
 </sst>
 </file>
@@ -320,9 +326,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,7 +647,7 @@
   <dimension ref="A1:A28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,142 +656,142 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>56</v>
       </c>
     </row>
@@ -795,10 +802,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6485A13F-7511-4C82-B2AF-6CE312822B9C}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,257 +816,315 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>58</v>
+      </c>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1070,10 +1135,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE426C38-4A9E-436E-90BD-D5812960D955}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,267 +1149,325 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>